<commit_message>
PB-LOG-025 cerrado + nuevo formato agregado para Gaselag + full drop area con modal
</commit_message>
<xml_diff>
--- a/backend/app/data/templates/logistica/LOG01_PLANTILLA_SALIDA.xlsx
+++ b/backend/app/data/templates/logistica/LOG01_PLANTILLA_SALIDA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\PROYECTO\PROJECT\MEDILESER_APP\backend\app\data\templates\logistica\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95A92F85-37C8-407C-B36C-BCF0265B246F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D27ED68D-63E3-4C50-889B-1BD98E7306DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -466,7 +466,7 @@
   <dimension ref="A1:P1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -475,7 +475,9 @@
     <col min="2" max="2" width="14.140625" customWidth="1"/>
     <col min="11" max="11" width="14.85546875" customWidth="1"/>
     <col min="12" max="12" width="12" customWidth="1"/>
-    <col min="15" max="15" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="7.85546875" customWidth="1"/>
+    <col min="15" max="15" width="12.28515625" customWidth="1"/>
+    <col min="16" max="16" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="28.5" x14ac:dyDescent="0.25">

</xml_diff>